<commit_message>
Card Swiping and Mosque data fixed
</commit_message>
<xml_diff>
--- a/assets/data/Recommendation/data/whole_data_cleaned.xlsx
+++ b/assets/data/Recommendation/data/whole_data_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\wayou-lt\assets\data\Recommendation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCAB801-0FC6-413D-843A-F934ADDB64AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6DB470-CBE5-460C-A186-DCC372EDD67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="15165" windowHeight="15015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3411,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4824,7 +4824,7 @@
         <v>261</v>
       </c>
       <c r="B49">
-        <v>4.9000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="C49">
         <v>868833</v>
@@ -5201,7 +5201,7 @@
         <v>333</v>
       </c>
       <c r="B62">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="C62">
         <v>777046</v>
@@ -5230,7 +5230,7 @@
         <v>338</v>
       </c>
       <c r="B63">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C63">
         <v>130835</v>
@@ -5491,7 +5491,7 @@
         <v>389</v>
       </c>
       <c r="B72">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="C72">
         <v>266340</v>
@@ -5549,7 +5549,7 @@
         <v>399</v>
       </c>
       <c r="B74">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C74">
         <v>653321</v>
@@ -5897,7 +5897,7 @@
         <v>467</v>
       </c>
       <c r="B86">
-        <v>4.9000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="C86">
         <v>776089</v>
@@ -5955,7 +5955,7 @@
         <v>477</v>
       </c>
       <c r="B88">
-        <v>4.7</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C88">
         <v>739809</v>
@@ -5984,7 +5984,7 @@
         <v>482</v>
       </c>
       <c r="B89">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C89">
         <v>360880</v>
@@ -6622,7 +6622,7 @@
         <v>596</v>
       </c>
       <c r="B111">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C111">
         <v>859308</v>
@@ -6651,7 +6651,7 @@
         <v>601</v>
       </c>
       <c r="B112">
-        <v>4.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C112">
         <v>260289</v>
@@ -6767,7 +6767,7 @@
         <v>622</v>
       </c>
       <c r="B116">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="C116">
         <v>213192</v>
@@ -6854,7 +6854,7 @@
         <v>638</v>
       </c>
       <c r="B119">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="C119">
         <v>221021</v>
@@ -6941,7 +6941,7 @@
         <v>654</v>
       </c>
       <c r="B122">
-        <v>4.5999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="C122">
         <v>879950</v>
@@ -6999,7 +6999,7 @@
         <v>664</v>
       </c>
       <c r="B124">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C124">
         <v>489599</v>
@@ -7057,7 +7057,7 @@
         <v>674</v>
       </c>
       <c r="B126">
-        <v>4.9000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="C126">
         <v>204226</v>
@@ -7405,7 +7405,7 @@
         <v>735</v>
       </c>
       <c r="B138">
-        <v>4.9000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="C138">
         <v>443705</v>
@@ -7463,7 +7463,7 @@
         <v>745</v>
       </c>
       <c r="B140">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="C140">
         <v>755016</v>
@@ -7492,7 +7492,7 @@
         <v>751</v>
       </c>
       <c r="B141">
-        <v>4.7</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C141">
         <v>708729</v>
@@ -7550,7 +7550,7 @@
         <v>762</v>
       </c>
       <c r="B143">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="C143">
         <v>516585</v>
@@ -7579,7 +7579,7 @@
         <v>767</v>
       </c>
       <c r="B144">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="C144">
         <v>897781</v>
@@ -7608,7 +7608,7 @@
         <v>773</v>
       </c>
       <c r="B145">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C145">
         <v>148271</v>
@@ -7666,7 +7666,7 @@
         <v>784</v>
       </c>
       <c r="B147">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="C147">
         <v>322220</v>
@@ -7695,7 +7695,7 @@
         <v>789</v>
       </c>
       <c r="B148">
-        <v>4.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C148">
         <v>563837</v>
@@ -7724,7 +7724,7 @@
         <v>794</v>
       </c>
       <c r="B149">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="C149">
         <v>554262</v>
@@ -7898,7 +7898,7 @@
         <v>826</v>
       </c>
       <c r="B155">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="C155">
         <v>928073</v>
@@ -8159,7 +8159,7 @@
         <v>875</v>
       </c>
       <c r="B164">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="C164">
         <v>274391</v>
@@ -8565,7 +8565,7 @@
         <v>948</v>
       </c>
       <c r="B178">
-        <v>4.7</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C178">
         <v>939682</v>
@@ -8710,7 +8710,7 @@
         <v>973</v>
       </c>
       <c r="B183">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C183">
         <v>661463</v>

</xml_diff>